<commit_message>
update django and add files
</commit_message>
<xml_diff>
--- a/大创/负责老师联系方式.xlsx
+++ b/大创/负责老师联系方式.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\03_大创实践\2018_第十一届\立项提交\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ShadowInk\大创\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>电子工程学院</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -186,10 +186,6 @@
   </si>
   <si>
     <t>韩康榕</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hankr@bupt.edu.cn</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -232,10 +228,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>zwxiu21@163.com</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>明光楼6</t>
     </r>
@@ -251,21 +243,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>科研楼1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>刁婷</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -392,12 +369,28 @@
     <t>教一楼309</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>you are so good.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hankr@bupt.edu.cn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zwxiu21@163.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>科研楼120</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -446,13 +439,62 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F200"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF905"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -544,18 +586,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -577,9 +619,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -604,9 +643,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -622,39 +658,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="已访问的超链接" xfId="1" builtinId="9"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFF905"/>
+      <color rgb="FFF7F604"/>
+      <color rgb="FFF8F200"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -953,378 +1058,418 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="26.75" style="10" customWidth="1"/>
-    <col min="4" max="4" width="36.875" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
+    <col min="3" max="3" width="46.3984375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="34.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:30" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:30" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="30" t="s">
+      <c r="B3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="C4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA4" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="26"/>
+      <c r="AD4" s="26"/>
+    </row>
+    <row r="5" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+    </row>
+    <row r="6" spans="1:30" ht="124.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+    </row>
+    <row r="7" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="26"/>
+    </row>
+    <row r="8" spans="1:30" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="26"/>
+      <c r="AD8" s="26"/>
+    </row>
+    <row r="9" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="31"/>
-      <c r="B4" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="C9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="26"/>
+    </row>
+    <row r="10" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA10" s="26"/>
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="26"/>
+      <c r="AD10" s="26"/>
+    </row>
+    <row r="11" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="34" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="C15" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+    </row>
+    <row r="16" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="27"/>
-      <c r="B6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="27"/>
-      <c r="B11" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="22" t="s">
+    <row r="31" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="27"/>
-      <c r="B13" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="B31" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="22" t="s">
+      <c r="C31" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="11"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="11"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="11"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="11"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="11"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="11"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="11"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="11"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="13"/>
-    </row>
-    <row r="25" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="11"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="11"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="1:4" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="11"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="29"/>
-      <c r="B29" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="22" t="s">
+      <c r="B32" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="C32" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="22" t="s">
+      <c r="B33" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="C33" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>63</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="AA4:AD10"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A12:A13"/>
@@ -1353,46 +1498,46 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>